<commit_message>
2018-09-06 models relations issues in migrations
</commit_message>
<xml_diff>
--- a/WMS/draft db.xlsx
+++ b/WMS/draft db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="120" windowWidth="11412" windowHeight="3432" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="120" windowWidth="11412" windowHeight="3432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>desc</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -502,23 +505,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -526,7 +532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -534,7 +540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -551,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>